<commit_message>
update 01 screening results for reviewer 1 with assignments for me and Jingxi
</commit_message>
<xml_diff>
--- a/01 Screening results NewPapers.xlsx
+++ b/01 Screening results NewPapers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\projects\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4563345F-401D-4927-A418-3BF4EBD0E12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C00EAD2-E1FF-4BBB-98B5-97A6E9872E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviewer1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="521">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -1578,6 +1578,15 @@
   </si>
   <si>
     <t>Workshop Preface</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Jérôme</t>
+  </si>
+  <si>
+    <t>Jingxi</t>
   </si>
 </sst>
 </file>
@@ -2447,2235 +2456,2514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:L94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11" style="3"/>
-    <col min="3" max="3" width="55.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="107.33203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="11" style="3"/>
+    <col min="4" max="4" width="55.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="107.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>519</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>519</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="1:13" ht="203" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>519</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>519</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:13" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>45</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>519</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>50</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+    <row r="10" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>519</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>54</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>55</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+    <row r="11" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>519</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>60</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>61</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="12" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>519</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>65</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>519</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
       <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
         <v>32</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>69</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>70</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>71</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="144" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
+    <row r="14" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>519</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
         <v>75</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>76</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
+    <row r="15" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>519</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>80</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>81</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>82</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
+    <row r="16" spans="1:13" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>519</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>86</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
+    <row r="17" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>519</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>90</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>91</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+    <row r="18" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>519</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E18" t="s">
-        <v>19</v>
-      </c>
       <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
         <v>32</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>95</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>96</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>97</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C19" s="2" t="s">
+    <row r="19" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>519</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
-        <v>19</v>
-      </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
         <v>101</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>102</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>103</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
+    <row r="20" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>519</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E20" t="s">
-        <v>19</v>
-      </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
         <v>21</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>107</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>108</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>519</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>112</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
+    <row r="22" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>519</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>116</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
+    <row r="23" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>519</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E23" t="s">
-        <v>19</v>
-      </c>
       <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
         <v>32</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>120</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>121</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>122</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
+    <row r="24" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>519</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
       <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
         <v>32</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>126</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>127</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>128</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
+    <row r="25" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>519</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
       <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
         <v>32</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>120</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>132</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>133</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C26" s="2" t="s">
+    <row r="26" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>519</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" t="s">
         <v>137</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C27" s="2" t="s">
+    <row r="27" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>519</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E27" t="s">
-        <v>19</v>
-      </c>
       <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="s">
         <v>32</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>141</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>142</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>143</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C28" s="2" t="s">
+    <row r="28" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>519</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
       <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
         <v>32</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>147</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>148</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>149</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C29" s="2" t="s">
+    <row r="29" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>519</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E29" t="s">
-        <v>19</v>
-      </c>
       <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
         <v>32</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>153</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>154</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>155</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C30" s="2" t="s">
+    <row r="30" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>519</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>32</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>159</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>160</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C31" s="2" t="s">
+    <row r="31" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>519</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E31" t="s">
-        <v>19</v>
-      </c>
       <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="s">
         <v>32</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>164</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>165</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>166</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C32" s="2" t="s">
+    <row r="32" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>519</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E32" t="s">
-        <v>19</v>
-      </c>
       <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
         <v>32</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>170</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>171</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>172</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C33" s="2" t="s">
+    <row r="33" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>519</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
       <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
         <v>32</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>33</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>176</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>177</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C34" s="2" t="s">
+    <row r="34" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>519</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>181</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>182</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C35" s="2" t="s">
+    <row r="35" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>519</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>181</v>
       </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
       <c r="G35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
         <v>186</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>187</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>188</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C36" s="2" t="s">
+    <row r="36" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>519</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E36" t="s">
-        <v>19</v>
-      </c>
       <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
         <v>192</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>193</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>194</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="3:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C37" s="2" t="s">
+    <row r="37" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>519</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E37" t="s">
-        <v>19</v>
-      </c>
       <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
         <v>32</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>198</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>199</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>200</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C38" s="2" t="s">
+    <row r="38" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>519</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E38" t="s">
-        <v>19</v>
-      </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
         <v>21</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>204</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>205</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C39" s="2" t="s">
+    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>519</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>209</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C40" s="2" t="s">
+    <row r="40" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>519</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>49</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C41" s="2" t="s">
+    <row r="41" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>519</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E41" t="s">
-        <v>19</v>
-      </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
         <v>216</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>217</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>218</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C42" s="2" t="s">
+    <row r="42" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>519</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G42" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" t="s">
         <v>222</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>223</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>224</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="3:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C43" s="2" t="s">
+    <row r="43" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>519</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>59</v>
       </c>
-      <c r="F43" t="s">
-        <v>20</v>
-      </c>
       <c r="G43" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" t="s">
         <v>228</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>229</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>230</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C44" s="2" t="s">
+    <row r="44" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>519</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>181</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>234</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>235</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>236</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="C45" s="2" t="s">
+    <row r="45" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>519</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
       <c r="F45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" t="s">
         <v>32</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>240</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>241</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>242</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C46" s="2" t="s">
+    <row r="46" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>519</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>181</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>246</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C47" s="2" t="s">
+    <row r="47" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>519</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>181</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>32</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>250</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>251</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>252</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="3:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="C48" s="2" t="s">
+    <row r="48" spans="1:11" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>519</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>256</v>
       </c>
-      <c r="F48" t="s">
-        <v>20</v>
-      </c>
       <c r="G48" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" t="s">
         <v>257</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>258</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>259</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C49" s="2" t="s">
+    <row r="49" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>520</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G49" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" t="s">
         <v>263</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>264</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>265</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C50" s="2" t="s">
+    <row r="50" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>520</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
       <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" t="s">
         <v>32</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>269</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>270</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="C51" s="2" t="s">
+    <row r="51" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>520</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E51" t="s">
-        <v>19</v>
-      </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G51" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" t="s">
         <v>21</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>274</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>275</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C52" s="2" t="s">
+    <row r="52" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>520</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>279</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C53" s="2" t="s">
+    <row r="53" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>520</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E53" t="s">
-        <v>19</v>
-      </c>
       <c r="F53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" t="s">
         <v>283</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>284</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>285</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="54" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C54" s="2" t="s">
+    <row r="54" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>520</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E54" t="s">
-        <v>19</v>
-      </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" t="s">
         <v>289</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>290</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="3:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C55" s="2" t="s">
+    <row r="55" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>520</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E55" t="s">
-        <v>19</v>
-      </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G55" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" t="s">
         <v>222</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>294</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>295</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C56" s="2" t="s">
+    <row r="56" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>520</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E56" t="s">
-        <v>19</v>
-      </c>
       <c r="F56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G56" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" t="s">
         <v>299</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>300</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>301</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C57" s="2" t="s">
+    <row r="57" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>520</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>305</v>
       </c>
-      <c r="F57" t="s">
-        <v>20</v>
-      </c>
       <c r="G57" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" t="s">
         <v>306</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>307</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>308</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="58" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C58" s="2" t="s">
+    <row r="58" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>520</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>256</v>
       </c>
-      <c r="F58" t="s">
-        <v>20</v>
-      </c>
       <c r="G58" t="s">
+        <v>20</v>
+      </c>
+      <c r="H58" t="s">
         <v>312</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>313</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C59" s="2" t="s">
+    <row r="59" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>520</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>305</v>
       </c>
-      <c r="F59" t="s">
-        <v>20</v>
-      </c>
       <c r="G59" t="s">
+        <v>20</v>
+      </c>
+      <c r="H59" t="s">
         <v>317</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>318</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>319</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C60" s="2" t="s">
+    <row r="60" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>520</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>181</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>32</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>269</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>323</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="61" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C61" s="2" t="s">
+    <row r="61" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>520</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E61" t="s">
-        <v>19</v>
-      </c>
       <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" t="s">
         <v>32</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>327</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>328</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>329</v>
       </c>
-      <c r="J61" t="s">
+      <c r="K61" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="62" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C62" s="2" t="s">
+    <row r="62" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>520</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>305</v>
       </c>
-      <c r="F62" t="s">
-        <v>20</v>
-      </c>
       <c r="G62" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" t="s">
         <v>317</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>333</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>334</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C63" s="2" t="s">
+    <row r="63" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>520</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>181</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>338</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>339</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="64" spans="3:10" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="C64" s="2" t="s">
+    <row r="64" spans="1:11" ht="203" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>520</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E64" t="s">
-        <v>19</v>
-      </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G64" t="s">
+        <v>20</v>
+      </c>
+      <c r="H64" t="s">
         <v>343</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>344</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>345</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="65" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C65" s="2" t="s">
+    <row r="65" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>520</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>256</v>
       </c>
-      <c r="F65" t="s">
-        <v>20</v>
-      </c>
       <c r="G65" t="s">
+        <v>20</v>
+      </c>
+      <c r="H65" t="s">
         <v>349</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>350</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>351</v>
       </c>
-      <c r="J65" t="s">
+      <c r="K65" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C66" s="2" t="s">
+    <row r="66" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>520</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>181</v>
       </c>
-      <c r="F66" t="s">
-        <v>20</v>
-      </c>
       <c r="G66" t="s">
+        <v>20</v>
+      </c>
+      <c r="H66" t="s">
         <v>355</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>356</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>357</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="67" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C67" s="2" t="s">
+    <row r="67" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>520</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="E67" t="s">
-        <v>19</v>
-      </c>
       <c r="F67" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" t="s">
         <v>32</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>95</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>361</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>362</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="3:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="C68" s="2" t="s">
+    <row r="68" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>520</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>256</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>32</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>366</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>367</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>368</v>
       </c>
-      <c r="J68" t="s">
+      <c r="K68" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C69" s="2" t="s">
+    <row r="69" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>520</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E69" t="s">
-        <v>19</v>
-      </c>
       <c r="F69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G69" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" t="s">
         <v>372</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>373</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
         <v>374</v>
       </c>
-      <c r="J69" t="s">
+      <c r="K69" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C70" s="2" t="s">
+    <row r="70" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>520</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>305</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>246</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="3:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C71" s="2" t="s">
+    <row r="71" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>520</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>305</v>
       </c>
-      <c r="F71" t="s">
-        <v>20</v>
-      </c>
       <c r="G71" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71" t="s">
         <v>381</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>382</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>383</v>
       </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="72" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C72" s="2" t="s">
+    <row r="72" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>520</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>181</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C73" s="2" t="s">
+    <row r="73" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>520</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="E73" t="s">
-        <v>19</v>
-      </c>
       <c r="F73" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" t="s">
         <v>32</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>389</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>390</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>391</v>
       </c>
-      <c r="J73" t="s">
+      <c r="K73" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="74" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C74" s="2" t="s">
+    <row r="74" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>520</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="E74" t="s">
-        <v>19</v>
-      </c>
       <c r="F74" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" t="s">
         <v>32</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>395</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>396</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>397</v>
       </c>
-      <c r="J74" t="s">
+      <c r="K74" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="75" spans="3:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C75" s="2" t="s">
+    <row r="75" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>520</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E75" t="s">
-        <v>19</v>
-      </c>
       <c r="F75" t="s">
+        <v>19</v>
+      </c>
+      <c r="G75" t="s">
         <v>32</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>401</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>402</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>403</v>
       </c>
-      <c r="J75" t="s">
+      <c r="K75" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="76" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C76" s="2" t="s">
+    <row r="76" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>520</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="E76" t="s">
-        <v>19</v>
-      </c>
       <c r="F76" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G76" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" t="s">
         <v>407</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>408</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>409</v>
       </c>
-      <c r="J76" t="s">
+      <c r="K76" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="77" spans="3:10" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="C77" s="2" t="s">
+    <row r="77" spans="1:11" ht="203" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>520</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>256</v>
       </c>
-      <c r="F77" t="s">
-        <v>20</v>
-      </c>
       <c r="G77" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" t="s">
         <v>283</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>413</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>414</v>
       </c>
-      <c r="J77" t="s">
+      <c r="K77" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="78" spans="3:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="C78" s="2" t="s">
+    <row r="78" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>520</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E78" t="s">
-        <v>19</v>
-      </c>
       <c r="F78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G78" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" t="s">
         <v>21</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>417</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>418</v>
       </c>
-      <c r="J78" t="s">
+      <c r="K78" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="79" spans="3:10" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="C79" s="2" t="s">
+    <row r="79" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>520</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="E79" t="s">
-        <v>19</v>
-      </c>
       <c r="F79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G79" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" t="s">
         <v>422</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>423</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>424</v>
       </c>
-      <c r="J79" t="s">
+      <c r="K79" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="80" spans="3:10" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C80" s="2" t="s">
+    <row r="80" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>520</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>428</v>
       </c>
-      <c r="J80" t="s">
+      <c r="K80" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C81" s="2" t="s">
+    <row r="81" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>520</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>59</v>
       </c>
-      <c r="F81" t="s">
-        <v>20</v>
-      </c>
       <c r="G81" t="s">
+        <v>20</v>
+      </c>
+      <c r="H81" t="s">
         <v>432</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>433</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>434</v>
       </c>
-      <c r="J81" t="s">
+      <c r="K81" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C82" s="2" t="s">
+    <row r="82" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>520</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="E82" t="s">
-        <v>19</v>
-      </c>
       <c r="F82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G82" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82" t="s">
         <v>101</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>438</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>439</v>
       </c>
-      <c r="J82" t="s">
+      <c r="K82" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C83" s="2" t="s">
+    <row r="83" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>520</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>59</v>
       </c>
-      <c r="F83" t="s">
-        <v>20</v>
-      </c>
       <c r="G83" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" t="s">
         <v>443</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>444</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>445</v>
       </c>
-      <c r="J83" t="s">
+      <c r="K83" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="84" spans="3:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="C84" s="2" t="s">
+    <row r="84" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>520</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="E84" t="s">
-        <v>19</v>
-      </c>
       <c r="F84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G84" t="s">
+        <v>20</v>
+      </c>
+      <c r="H84" t="s">
         <v>263</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>449</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>450</v>
       </c>
-      <c r="J84" t="s">
+      <c r="K84" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="85" spans="3:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="C85" s="2" t="s">
+    <row r="85" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>520</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>454</v>
       </c>
-      <c r="J85" t="s">
+      <c r="K85" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="3:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C86" s="2" t="s">
+    <row r="86" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>520</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>305</v>
       </c>
-      <c r="F86" t="s">
-        <v>20</v>
-      </c>
       <c r="G86" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" t="s">
         <v>458</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>459</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>460</v>
       </c>
-      <c r="J86" t="s">
+      <c r="K86" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C87" s="2" t="s">
+    <row r="87" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>520</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="E87" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>181</v>
       </c>
-      <c r="F87" t="s">
-        <v>20</v>
-      </c>
       <c r="G87" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" t="s">
         <v>464</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>465</v>
       </c>
-      <c r="I87" t="s">
+      <c r="J87" t="s">
         <v>466</v>
       </c>
-      <c r="J87" t="s">
+      <c r="K87" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="88" spans="3:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C88" s="2" t="s">
+    <row r="88" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>520</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>181</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>32</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>470</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>471</v>
       </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>472</v>
       </c>
-      <c r="J88" t="s">
+      <c r="K88" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="89" spans="3:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="C89" s="2" t="s">
+    <row r="89" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>520</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>256</v>
       </c>
-      <c r="F89" t="s">
-        <v>20</v>
-      </c>
       <c r="G89" t="s">
+        <v>20</v>
+      </c>
+      <c r="H89" t="s">
         <v>476</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>477</v>
       </c>
-      <c r="I89" t="s">
+      <c r="J89" t="s">
         <v>478</v>
       </c>
-      <c r="J89" t="s">
+      <c r="K89" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="90" spans="3:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="C90" s="2" t="s">
+    <row r="90" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>520</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="E90" t="s">
-        <v>19</v>
-      </c>
       <c r="F90" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" t="s">
         <v>32</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>389</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>482</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
         <v>483</v>
       </c>
-      <c r="J90" t="s">
+      <c r="K90" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="91" spans="3:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="C91" s="2" t="s">
+    <row r="91" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>520</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="E91" t="s">
-        <v>19</v>
-      </c>
       <c r="F91" t="s">
+        <v>19</v>
+      </c>
+      <c r="G91" t="s">
         <v>32</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>389</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>487</v>
       </c>
-      <c r="I91" t="s">
+      <c r="J91" t="s">
         <v>488</v>
       </c>
-      <c r="J91" t="s">
+      <c r="K91" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="92" spans="3:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="C92" s="2" t="s">
+    <row r="92" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>520</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>492</v>
       </c>
-      <c r="F92" t="s">
-        <v>20</v>
-      </c>
       <c r="G92" t="s">
+        <v>20</v>
+      </c>
+      <c r="H92" t="s">
         <v>493</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>494</v>
       </c>
-      <c r="I92" t="s">
+      <c r="J92" t="s">
         <v>495</v>
       </c>
-      <c r="J92" t="s">
+      <c r="K92" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="93" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="2" t="s">
+    <row r="93" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>520</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
       <c r="F93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G93" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" t="s">
         <v>21</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>499</v>
       </c>
-      <c r="I93" t="s">
+      <c r="J93" t="s">
         <v>500</v>
       </c>
-      <c r="J93" t="s">
+      <c r="K93" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="94" spans="3:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="C94" s="2" t="s">
+    <row r="94" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>520</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="E94" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="E94" t="s">
-        <v>19</v>
-      </c>
       <c r="F94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G94" t="s">
+        <v>20</v>
+      </c>
+      <c r="H94" t="s">
         <v>21</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>504</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>505</v>
       </c>
-      <c r="J94" t="s">
+      <c r="K94" t="s">
         <v>506</v>
       </c>
     </row>
@@ -4688,17 +4976,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="105.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="105.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4706,7 +4994,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -4744,7 +5032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>507</v>
       </c>
@@ -4762,7 +5050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>507</v>
       </c>
@@ -4794,7 +5082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="174" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>507</v>
       </c>
@@ -4818,7 +5106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="203" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>507</v>
       </c>
@@ -4848,7 +5136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>507</v>
       </c>
@@ -4878,7 +5166,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>509</v>
       </c>
@@ -4908,7 +5196,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>507</v>
       </c>
@@ -4935,7 +5223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>507</v>
       </c>
@@ -4965,7 +5253,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>507</v>
       </c>
@@ -4989,7 +5277,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>507</v>
       </c>
@@ -5007,7 +5295,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>507</v>
       </c>
@@ -5037,7 +5325,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="145" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>507</v>
       </c>
@@ -5061,7 +5349,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="116" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>507</v>
       </c>
@@ -5091,7 +5379,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
@@ -5107,7 +5395,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>509</v>
       </c>
@@ -5137,7 +5425,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>507</v>
       </c>
@@ -5167,7 +5455,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>507</v>
       </c>
@@ -5197,7 +5485,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>507</v>
       </c>
@@ -5229,7 +5517,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>507</v>
       </c>
@@ -5247,7 +5535,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>507</v>
       </c>
@@ -5265,7 +5553,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>507</v>
       </c>
@@ -5295,7 +5583,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>507</v>
       </c>
@@ -5325,7 +5613,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>507</v>
       </c>
@@ -5355,7 +5643,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>507</v>
       </c>
@@ -5376,7 +5664,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>507</v>
       </c>
@@ -5406,7 +5694,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>507</v>
       </c>
@@ -5436,7 +5724,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>507</v>
       </c>
@@ -5466,7 +5754,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>507</v>
       </c>
@@ -5493,7 +5781,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>511</v>
       </c>
@@ -5523,7 +5811,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>507</v>
       </c>
@@ -5553,7 +5841,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>507</v>
       </c>
@@ -5583,7 +5871,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>511</v>
       </c>
@@ -5604,7 +5892,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>511</v>
       </c>
@@ -5634,7 +5922,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>509</v>
       </c>
@@ -5661,7 +5949,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>507</v>
       </c>
@@ -5691,7 +5979,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>507</v>
       </c>
@@ -5723,7 +6011,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>507</v>
       </c>
@@ -5741,7 +6029,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>507</v>
       </c>
@@ -5759,7 +6047,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>507</v>
       </c>
@@ -5789,7 +6077,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>507</v>
       </c>
@@ -5819,7 +6107,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>507</v>
       </c>
@@ -5849,7 +6137,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>507</v>
       </c>
@@ -5876,7 +6164,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>511</v>
       </c>
@@ -5906,7 +6194,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>507</v>
       </c>
@@ -5927,7 +6215,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>507</v>
       </c>
@@ -5957,7 +6245,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="290" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="2" t="s">
@@ -5985,7 +6273,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>507</v>
       </c>
@@ -6015,7 +6303,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>507</v>
       </c>
@@ -6042,7 +6330,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>507</v>
       </c>
@@ -6072,7 +6360,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>507</v>
       </c>
@@ -6090,7 +6378,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>513</v>
       </c>
@@ -6120,7 +6408,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>514</v>
       </c>
@@ -6147,7 +6435,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>507</v>
       </c>
@@ -6177,7 +6465,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>507</v>
       </c>
@@ -6207,7 +6495,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>507</v>
       </c>
@@ -6237,7 +6525,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>507</v>
       </c>
@@ -6264,7 +6552,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>507</v>
       </c>
@@ -6294,7 +6582,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>507</v>
       </c>
@@ -6323,7 +6611,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>507</v>
       </c>
@@ -6353,7 +6641,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>511</v>
       </c>
@@ -6383,7 +6671,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>507</v>
       </c>
@@ -6407,7 +6695,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="203" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>507</v>
       </c>
@@ -6437,7 +6725,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>514</v>
       </c>
@@ -6467,7 +6755,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>507</v>
       </c>
@@ -6497,7 +6785,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>507</v>
       </c>
@@ -6527,7 +6815,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>507</v>
       </c>
@@ -6557,7 +6845,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>507</v>
       </c>
@@ -6587,7 +6875,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>507</v>
       </c>
@@ -6608,7 +6896,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>507</v>
       </c>
@@ -6638,7 +6926,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>516</v>
       </c>
@@ -6658,7 +6946,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>507</v>
       </c>
@@ -6688,7 +6976,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>507</v>
       </c>
@@ -6718,7 +7006,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>507</v>
       </c>
@@ -6748,7 +7036,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>507</v>
       </c>
@@ -6778,7 +7066,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>513</v>
       </c>
@@ -6808,7 +7096,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>509</v>
       </c>
@@ -6838,7 +7126,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="174" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>507</v>
       </c>
@@ -6868,7 +7156,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>507</v>
       </c>
@@ -6886,7 +7174,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>507</v>
       </c>
@@ -6916,7 +7204,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>507</v>
       </c>
@@ -6946,7 +7234,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>511</v>
       </c>
@@ -6976,7 +7264,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>514</v>
       </c>
@@ -7006,7 +7294,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>507</v>
       </c>
@@ -7024,7 +7312,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>507</v>
       </c>
@@ -7054,7 +7342,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>507</v>
       </c>
@@ -7084,7 +7372,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>507</v>
       </c>
@@ -7114,7 +7402,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>507</v>
       </c>
@@ -7144,7 +7432,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>507</v>
       </c>
@@ -7174,7 +7462,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="145" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>507</v>
       </c>
@@ -7204,7 +7492,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>507</v>
       </c>
@@ -7234,7 +7522,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>507</v>
       </c>
@@ -7264,7 +7552,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>507</v>
       </c>

</xml_diff>

<commit_message>
screening finished by me
</commit_message>
<xml_diff>
--- a/01 Screening results NewPapers.xlsx
+++ b/01 Screening results NewPapers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\projects\mde4dts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C00EAD2-E1FF-4BBB-98B5-97A6E9872E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183C70F7-72B0-43CF-AF3B-F9C3DA16931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="538">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -1587,6 +1587,57 @@
   </si>
   <si>
     <t>Jingxi</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>predictive model</t>
+  </si>
+  <si>
+    <t>simulating BP models</t>
+  </si>
+  <si>
+    <t>von uns :D</t>
+  </si>
+  <si>
+    <t>Daniels Diss</t>
+  </si>
+  <si>
+    <t>no DT</t>
+  </si>
+  <si>
+    <t>nicht sicher ob wirklich MDE</t>
+  </si>
+  <si>
+    <t>secondary study</t>
+  </si>
+  <si>
+    <t>no DT?</t>
+  </si>
+  <si>
+    <t>no MDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sie haben ein Modell und nennen ihr modellverarbeitendes Tool DT </t>
+  </si>
+  <si>
+    <t>experience</t>
+  </si>
+  <si>
+    <t>mathematical model</t>
+  </si>
+  <si>
+    <t>challenges</t>
+  </si>
+  <si>
+    <t>Titel vs. Abstract?</t>
+  </si>
+  <si>
+    <t>no MDE, no DT</t>
+  </si>
+  <si>
+    <t>no MDE + no DT</t>
   </si>
 </sst>
 </file>
@@ -2458,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2519,6 +2570,12 @@
       <c r="A3" t="s">
         <v>519</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>522</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2536,6 +2593,9 @@
       <c r="A4" t="s">
         <v>519</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2565,6 +2625,12 @@
       <c r="A5" t="s">
         <v>519</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>523</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2588,6 +2654,9 @@
       <c r="A6" t="s">
         <v>519</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
@@ -2617,6 +2686,12 @@
       <c r="A7" t="s">
         <v>519</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>524</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
@@ -2646,6 +2721,12 @@
       <c r="A8" t="s">
         <v>519</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>525</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2675,6 +2756,9 @@
       <c r="A9" t="s">
         <v>519</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
@@ -2701,6 +2785,9 @@
       <c r="A10" t="s">
         <v>519</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
@@ -2730,6 +2817,9 @@
       <c r="A11" t="s">
         <v>519</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
@@ -2753,6 +2843,9 @@
       <c r="A12" t="s">
         <v>519</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
@@ -2770,6 +2863,12 @@
       <c r="A13" t="s">
         <v>519</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>527</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
@@ -2799,6 +2898,9 @@
       <c r="A14" t="s">
         <v>519</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>528</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
@@ -2822,6 +2924,12 @@
       <c r="A15" t="s">
         <v>519</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>529</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>78</v>
       </c>
@@ -2851,6 +2959,12 @@
       <c r="A16" t="s">
         <v>519</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>529</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>84</v>
       </c>
@@ -2868,6 +2982,9 @@
       <c r="A17" t="s">
         <v>519</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>530</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
@@ -2897,6 +3014,9 @@
       <c r="A18" t="s">
         <v>519</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>93</v>
       </c>
@@ -2926,6 +3046,9 @@
       <c r="A19" t="s">
         <v>519</v>
       </c>
+      <c r="B19" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>99</v>
       </c>
@@ -2955,6 +3078,9 @@
       <c r="A20" t="s">
         <v>519</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
@@ -2984,6 +3110,9 @@
       <c r="A21" t="s">
         <v>519</v>
       </c>
+      <c r="B21" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
@@ -3001,6 +3130,9 @@
       <c r="A22" t="s">
         <v>519</v>
       </c>
+      <c r="B22" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>114</v>
       </c>
@@ -3018,6 +3150,12 @@
       <c r="A23" t="s">
         <v>519</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>531</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>118</v>
       </c>
@@ -3047,6 +3185,9 @@
       <c r="A24" t="s">
         <v>519</v>
       </c>
+      <c r="B24" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
@@ -3076,6 +3217,9 @@
       <c r="A25" t="s">
         <v>519</v>
       </c>
+      <c r="B25" s="3" t="s">
+        <v>532</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>130</v>
       </c>
@@ -3105,6 +3249,9 @@
       <c r="A26" t="s">
         <v>519</v>
       </c>
+      <c r="B26" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>135</v>
       </c>
@@ -3125,6 +3272,9 @@
       <c r="A27" t="s">
         <v>519</v>
       </c>
+      <c r="B27" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>139</v>
       </c>
@@ -3154,6 +3304,9 @@
       <c r="A28" t="s">
         <v>519</v>
       </c>
+      <c r="B28" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>145</v>
       </c>
@@ -3183,6 +3336,9 @@
       <c r="A29" t="s">
         <v>519</v>
       </c>
+      <c r="B29" s="3" t="s">
+        <v>530</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>151</v>
       </c>
@@ -3212,6 +3368,12 @@
       <c r="A30" t="s">
         <v>519</v>
       </c>
+      <c r="B30" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>533</v>
+      </c>
       <c r="D30" s="2" t="s">
         <v>157</v>
       </c>
@@ -3238,6 +3400,9 @@
       <c r="A31" t="s">
         <v>519</v>
       </c>
+      <c r="B31" s="3" t="s">
+        <v>532</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>162</v>
       </c>
@@ -3267,6 +3432,9 @@
       <c r="A32" t="s">
         <v>519</v>
       </c>
+      <c r="B32" s="3" t="s">
+        <v>530</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>168</v>
       </c>
@@ -3296,6 +3464,9 @@
       <c r="A33" t="s">
         <v>519</v>
       </c>
+      <c r="B33" s="3" t="s">
+        <v>534</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>174</v>
       </c>
@@ -3325,6 +3496,9 @@
       <c r="A34" t="s">
         <v>519</v>
       </c>
+      <c r="B34" s="3" t="s">
+        <v>535</v>
+      </c>
       <c r="D34" s="2" t="s">
         <v>179</v>
       </c>
@@ -3345,6 +3519,9 @@
       <c r="A35" t="s">
         <v>519</v>
       </c>
+      <c r="B35" s="3" t="s">
+        <v>536</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>184</v>
       </c>
@@ -3374,6 +3551,9 @@
       <c r="A36" t="s">
         <v>519</v>
       </c>
+      <c r="B36" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>190</v>
       </c>
@@ -3400,6 +3580,9 @@
       <c r="A37" t="s">
         <v>519</v>
       </c>
+      <c r="B37" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>196</v>
       </c>
@@ -3429,6 +3612,9 @@
       <c r="A38" t="s">
         <v>519</v>
       </c>
+      <c r="B38" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>202</v>
       </c>
@@ -3458,6 +3644,9 @@
       <c r="A39" t="s">
         <v>519</v>
       </c>
+      <c r="B39" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>207</v>
       </c>
@@ -3475,6 +3664,12 @@
       <c r="A40" t="s">
         <v>519</v>
       </c>
+      <c r="B40" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>529</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>211</v>
       </c>
@@ -3492,6 +3687,9 @@
       <c r="A41" t="s">
         <v>519</v>
       </c>
+      <c r="B41" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>214</v>
       </c>
@@ -3521,6 +3719,9 @@
       <c r="A42" t="s">
         <v>519</v>
       </c>
+      <c r="B42" s="3" t="s">
+        <v>521</v>
+      </c>
       <c r="D42" s="2" t="s">
         <v>220</v>
       </c>
@@ -3550,6 +3751,9 @@
       <c r="A43" t="s">
         <v>519</v>
       </c>
+      <c r="B43" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>226</v>
       </c>
@@ -3579,6 +3783,12 @@
       <c r="A44" t="s">
         <v>519</v>
       </c>
+      <c r="B44" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>529</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>232</v>
       </c>
@@ -3605,6 +3815,9 @@
       <c r="A45" t="s">
         <v>519</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>537</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>238</v>
       </c>
@@ -3634,6 +3847,12 @@
       <c r="A46" t="s">
         <v>519</v>
       </c>
+      <c r="B46" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>529</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>244</v>
       </c>
@@ -3654,6 +3873,9 @@
       <c r="A47" t="s">
         <v>519</v>
       </c>
+      <c r="B47" s="3" t="s">
+        <v>532</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>248</v>
       </c>
@@ -3682,6 +3904,12 @@
     <row r="48" spans="1:11" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>519</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>529</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>254</v>
@@ -4976,8 +5204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update files with new papers
</commit_message>
<xml_diff>
--- a/01 Screening results NewPapers.xlsx
+++ b/01 Screening results NewPapers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCE093A-1B37-4731-B0F1-B3A7A924D241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270D1BAC-A7EE-4A03-B54F-E9A03EC4DBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reviewer1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tabelle1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Reviewer2!$A$1:$N$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Reviewer2!$A$1:$K$94</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="559">
   <si>
     <t>Reviewer 1</t>
   </si>
@@ -2586,23 +2586,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="11" style="3"/>
-    <col min="4" max="4" width="55.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="107.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="107.44140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>518</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>519</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>519</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>519</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="225" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>519</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>519</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>519</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>519</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>519</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>519</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>519</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>519</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>519</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>519</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>519</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>519</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>519</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>519</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>519</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>519</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>519</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>519</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>519</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>519</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>519</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>519</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>519</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>519</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>519</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>519</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>519</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>519</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>519</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>519</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>519</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>519</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>519</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>519</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>519</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>519</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>519</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>519</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>519</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>519</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>519</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>519</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>519</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>520</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>520</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>520</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>520</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>520</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>520</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>520</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>520</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>520</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>520</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>520</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>520</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>520</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>520</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>520</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>520</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>520</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>520</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>520</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>520</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>520</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>520</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>520</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>520</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>520</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>520</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>520</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>520</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>520</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>520</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>520</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>520</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>520</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>520</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>520</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>520</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>520</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>520</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>520</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>520</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>520</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>520</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>520</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>520</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>520</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>520</v>
       </c>
@@ -5489,20 +5489,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E94"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E93" sqref="A93:E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="48" customWidth="1"/>
-    <col min="6" max="6" width="105.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="105.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>556</v>
       </c>
@@ -5516,7 +5515,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5530,31 +5529,19 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>507</v>
       </c>
@@ -5572,14 +5559,14 @@
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>507</v>
       </c>
@@ -5600,25 +5587,19 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>507</v>
       </c>
@@ -5637,19 +5618,16 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>507</v>
       </c>
@@ -5668,25 +5646,19 @@
         <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
         <v>32</v>
       </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>507</v>
       </c>
@@ -5705,25 +5677,19 @@
         <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>507</v>
       </c>
@@ -5742,25 +5708,19 @@
         <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>507</v>
       </c>
@@ -5779,22 +5739,19 @@
         <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
         <v>20</v>
       </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>507</v>
       </c>
@@ -5813,25 +5770,19 @@
         <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
         <v>20</v>
       </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>507</v>
       </c>
@@ -5850,19 +5801,16 @@
         <v>58</v>
       </c>
       <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>507</v>
       </c>
@@ -5880,14 +5828,14 @@
       <c r="F12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I12" t="s">
+      <c r="G12" t="s">
         <v>65</v>
       </c>
-      <c r="L12" t="s">
+      <c r="H12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>507</v>
       </c>
@@ -5906,25 +5854,19 @@
         <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" t="s">
-        <v>70</v>
-      </c>
-      <c r="K13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>528</v>
       </c>
@@ -5944,19 +5886,16 @@
         <v>74</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" t="s">
-        <v>76</v>
-      </c>
-      <c r="L14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>507</v>
       </c>
@@ -5975,25 +5914,19 @@
         <v>79</v>
       </c>
       <c r="G15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" t="s">
         <v>59</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K15" t="s">
         <v>32</v>
       </c>
-      <c r="I15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" t="s">
-        <v>82</v>
-      </c>
-      <c r="L15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>507</v>
       </c>
@@ -6009,14 +5942,14 @@
       <c r="F16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I16" t="s">
+      <c r="G16" t="s">
         <v>86</v>
       </c>
-      <c r="L16" t="s">
+      <c r="H16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>557</v>
       </c>
@@ -6035,25 +5968,19 @@
         <v>89</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
         <v>20</v>
       </c>
-      <c r="I17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>507</v>
       </c>
@@ -6072,25 +5999,19 @@
         <v>94</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s">
         <v>32</v>
       </c>
-      <c r="I18" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" t="s">
-        <v>96</v>
-      </c>
-      <c r="K18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>507</v>
       </c>
@@ -6109,25 +6030,19 @@
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
         <v>20</v>
       </c>
-      <c r="I19" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" t="s">
-        <v>103</v>
-      </c>
-      <c r="L19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>507</v>
       </c>
@@ -6148,25 +6063,19 @@
         <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" t="s">
         <v>20</v>
       </c>
-      <c r="I20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" t="s">
-        <v>107</v>
-      </c>
-      <c r="K20" t="s">
-        <v>108</v>
-      </c>
-      <c r="L20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>507</v>
       </c>
@@ -6184,14 +6093,14 @@
       <c r="F21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I21" t="s">
+      <c r="G21" t="s">
         <v>112</v>
       </c>
-      <c r="L21" t="s">
+      <c r="H21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>507</v>
       </c>
@@ -6209,14 +6118,14 @@
       <c r="F22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I22" t="s">
+      <c r="G22" t="s">
         <v>116</v>
       </c>
-      <c r="L22" t="s">
+      <c r="H22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>507</v>
       </c>
@@ -6235,25 +6144,19 @@
         <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="H23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" t="s">
         <v>32</v>
       </c>
-      <c r="I23" t="s">
-        <v>120</v>
-      </c>
-      <c r="J23" t="s">
-        <v>121</v>
-      </c>
-      <c r="K23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>507</v>
       </c>
@@ -6272,25 +6175,19 @@
         <v>125</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="H24" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" t="s">
         <v>32</v>
       </c>
-      <c r="I24" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" t="s">
-        <v>127</v>
-      </c>
-      <c r="K24" t="s">
-        <v>128</v>
-      </c>
-      <c r="L24" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>507</v>
       </c>
@@ -6309,25 +6206,19 @@
         <v>131</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="H25" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" t="s">
         <v>32</v>
       </c>
-      <c r="I25" t="s">
-        <v>120</v>
-      </c>
-      <c r="J25" t="s">
-        <v>132</v>
-      </c>
-      <c r="K25" t="s">
-        <v>133</v>
-      </c>
-      <c r="L25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>507</v>
       </c>
@@ -6346,16 +6237,16 @@
         <v>136</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>137</v>
+      </c>
+      <c r="H26" t="s">
+        <v>138</v>
       </c>
       <c r="I26" t="s">
-        <v>137</v>
-      </c>
-      <c r="L26" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>507</v>
       </c>
@@ -6374,25 +6265,19 @@
         <v>140</v>
       </c>
       <c r="G27" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="H27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" t="s">
         <v>32</v>
       </c>
-      <c r="I27" t="s">
-        <v>141</v>
-      </c>
-      <c r="J27" t="s">
-        <v>142</v>
-      </c>
-      <c r="K27" t="s">
-        <v>143</v>
-      </c>
-      <c r="L27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>507</v>
       </c>
@@ -6411,25 +6296,19 @@
         <v>146</v>
       </c>
       <c r="G28" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="H28" t="s">
+        <v>150</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" t="s">
         <v>32</v>
       </c>
-      <c r="I28" t="s">
-        <v>147</v>
-      </c>
-      <c r="J28" t="s">
-        <v>148</v>
-      </c>
-      <c r="K28" t="s">
-        <v>149</v>
-      </c>
-      <c r="L28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>507</v>
       </c>
@@ -6448,25 +6327,19 @@
         <v>152</v>
       </c>
       <c r="G29" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="H29" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" t="s">
         <v>32</v>
       </c>
-      <c r="I29" t="s">
-        <v>153</v>
-      </c>
-      <c r="J29" t="s">
-        <v>154</v>
-      </c>
-      <c r="K29" t="s">
-        <v>155</v>
-      </c>
-      <c r="L29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>507</v>
       </c>
@@ -6485,22 +6358,19 @@
         <v>158</v>
       </c>
       <c r="G30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30" t="s">
         <v>59</v>
       </c>
-      <c r="H30" t="s">
+      <c r="K30" t="s">
         <v>32</v>
       </c>
-      <c r="I30" t="s">
-        <v>159</v>
-      </c>
-      <c r="J30" t="s">
-        <v>160</v>
-      </c>
-      <c r="L30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>532</v>
       </c>
@@ -6519,25 +6389,19 @@
         <v>163</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="H31" t="s">
+        <v>167</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" t="s">
         <v>32</v>
       </c>
-      <c r="I31" t="s">
-        <v>164</v>
-      </c>
-      <c r="J31" t="s">
-        <v>165</v>
-      </c>
-      <c r="K31" t="s">
-        <v>166</v>
-      </c>
-      <c r="L31" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>507</v>
       </c>
@@ -6556,25 +6420,19 @@
         <v>169</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="H32" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" t="s">
         <v>32</v>
       </c>
-      <c r="I32" t="s">
-        <v>170</v>
-      </c>
-      <c r="J32" t="s">
-        <v>171</v>
-      </c>
-      <c r="K32" t="s">
-        <v>172</v>
-      </c>
-      <c r="L32" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>507</v>
       </c>
@@ -6593,25 +6451,19 @@
         <v>175</v>
       </c>
       <c r="G33" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" t="s">
         <v>32</v>
       </c>
-      <c r="I33" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" t="s">
-        <v>176</v>
-      </c>
-      <c r="K33" t="s">
-        <v>177</v>
-      </c>
-      <c r="L33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>511</v>
       </c>
@@ -6630,16 +6482,16 @@
         <v>180</v>
       </c>
       <c r="G34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" t="s">
+        <v>183</v>
+      </c>
+      <c r="I34" t="s">
         <v>181</v>
       </c>
-      <c r="I34" t="s">
-        <v>182</v>
-      </c>
-      <c r="L34" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>511</v>
       </c>
@@ -6658,25 +6510,19 @@
         <v>185</v>
       </c>
       <c r="G35" t="s">
+        <v>186</v>
+      </c>
+      <c r="H35" t="s">
+        <v>189</v>
+      </c>
+      <c r="I35" t="s">
         <v>181</v>
       </c>
-      <c r="H35" t="s">
+      <c r="K35" t="s">
         <v>20</v>
       </c>
-      <c r="I35" t="s">
-        <v>186</v>
-      </c>
-      <c r="J35" t="s">
-        <v>187</v>
-      </c>
-      <c r="K35" t="s">
-        <v>188</v>
-      </c>
-      <c r="L35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>557</v>
       </c>
@@ -6695,22 +6541,19 @@
         <v>191</v>
       </c>
       <c r="G36" t="s">
-        <v>19</v>
+        <v>193</v>
       </c>
       <c r="H36" t="s">
+        <v>195</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" t="s">
         <v>192</v>
       </c>
-      <c r="I36" t="s">
-        <v>193</v>
-      </c>
-      <c r="J36" t="s">
-        <v>194</v>
-      </c>
-      <c r="L36" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>507</v>
       </c>
@@ -6729,25 +6572,19 @@
         <v>197</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="H37" t="s">
+        <v>201</v>
+      </c>
+      <c r="I37" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" t="s">
         <v>32</v>
       </c>
-      <c r="I37" t="s">
-        <v>198</v>
-      </c>
-      <c r="J37" t="s">
-        <v>199</v>
-      </c>
-      <c r="K37" t="s">
-        <v>200</v>
-      </c>
-      <c r="L37" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>507</v>
       </c>
@@ -6768,25 +6605,19 @@
         <v>203</v>
       </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H38" t="s">
+        <v>206</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" t="s">
         <v>20</v>
       </c>
-      <c r="I38" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" t="s">
-        <v>204</v>
-      </c>
-      <c r="K38" t="s">
-        <v>205</v>
-      </c>
-      <c r="L38" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>507</v>
       </c>
@@ -6804,14 +6635,14 @@
       <c r="F39" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="I39" t="s">
+      <c r="G39" t="s">
         <v>209</v>
       </c>
-      <c r="L39" t="s">
+      <c r="H39" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>507</v>
       </c>
@@ -6829,14 +6660,14 @@
       <c r="F40" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="I40" t="s">
+      <c r="G40" t="s">
         <v>49</v>
       </c>
-      <c r="L40" t="s">
+      <c r="H40" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>507</v>
       </c>
@@ -6855,25 +6686,19 @@
         <v>215</v>
       </c>
       <c r="G41" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
       <c r="H41" t="s">
+        <v>219</v>
+      </c>
+      <c r="I41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" t="s">
         <v>20</v>
       </c>
-      <c r="I41" t="s">
-        <v>216</v>
-      </c>
-      <c r="J41" t="s">
-        <v>217</v>
-      </c>
-      <c r="K41" t="s">
-        <v>218</v>
-      </c>
-      <c r="L41" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>507</v>
       </c>
@@ -6892,25 +6717,19 @@
         <v>221</v>
       </c>
       <c r="G42" t="s">
-        <v>19</v>
+        <v>222</v>
       </c>
       <c r="H42" t="s">
+        <v>225</v>
+      </c>
+      <c r="I42" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" t="s">
         <v>20</v>
       </c>
-      <c r="I42" t="s">
-        <v>222</v>
-      </c>
-      <c r="J42" t="s">
-        <v>223</v>
-      </c>
-      <c r="K42" t="s">
-        <v>224</v>
-      </c>
-      <c r="L42" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>507</v>
       </c>
@@ -6929,25 +6748,19 @@
         <v>227</v>
       </c>
       <c r="G43" t="s">
+        <v>228</v>
+      </c>
+      <c r="H43" t="s">
+        <v>231</v>
+      </c>
+      <c r="I43" t="s">
         <v>59</v>
       </c>
-      <c r="H43" t="s">
+      <c r="K43" t="s">
         <v>20</v>
       </c>
-      <c r="I43" t="s">
-        <v>228</v>
-      </c>
-      <c r="J43" t="s">
-        <v>229</v>
-      </c>
-      <c r="K43" t="s">
-        <v>230</v>
-      </c>
-      <c r="L43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>507</v>
       </c>
@@ -6966,22 +6779,19 @@
         <v>233</v>
       </c>
       <c r="G44" t="s">
+        <v>235</v>
+      </c>
+      <c r="H44" t="s">
+        <v>237</v>
+      </c>
+      <c r="I44" t="s">
         <v>181</v>
       </c>
-      <c r="H44" t="s">
+      <c r="K44" t="s">
         <v>234</v>
       </c>
-      <c r="I44" t="s">
-        <v>235</v>
-      </c>
-      <c r="K44" t="s">
-        <v>236</v>
-      </c>
-      <c r="L44" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>511</v>
       </c>
@@ -7000,25 +6810,19 @@
         <v>239</v>
       </c>
       <c r="G45" t="s">
-        <v>19</v>
+        <v>240</v>
       </c>
       <c r="H45" t="s">
+        <v>243</v>
+      </c>
+      <c r="I45" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" t="s">
         <v>32</v>
       </c>
-      <c r="I45" t="s">
-        <v>240</v>
-      </c>
-      <c r="J45" t="s">
-        <v>241</v>
-      </c>
-      <c r="K45" t="s">
-        <v>242</v>
-      </c>
-      <c r="L45" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>507</v>
       </c>
@@ -7037,16 +6841,16 @@
         <v>245</v>
       </c>
       <c r="G46" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" t="s">
+        <v>247</v>
+      </c>
+      <c r="I46" t="s">
         <v>181</v>
       </c>
-      <c r="I46" t="s">
-        <v>246</v>
-      </c>
-      <c r="L46" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>507</v>
       </c>
@@ -7065,25 +6869,19 @@
         <v>249</v>
       </c>
       <c r="G47" t="s">
+        <v>250</v>
+      </c>
+      <c r="H47" t="s">
+        <v>253</v>
+      </c>
+      <c r="I47" t="s">
         <v>181</v>
       </c>
-      <c r="H47" t="s">
+      <c r="K47" t="s">
         <v>32</v>
       </c>
-      <c r="I47" t="s">
-        <v>250</v>
-      </c>
-      <c r="J47" t="s">
-        <v>251</v>
-      </c>
-      <c r="K47" t="s">
-        <v>252</v>
-      </c>
-      <c r="L47" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>507</v>
       </c>
@@ -7100,25 +6898,19 @@
         <v>255</v>
       </c>
       <c r="G48" t="s">
+        <v>257</v>
+      </c>
+      <c r="H48" t="s">
+        <v>260</v>
+      </c>
+      <c r="I48" t="s">
         <v>256</v>
       </c>
-      <c r="H48" t="s">
+      <c r="K48" t="s">
         <v>20</v>
       </c>
-      <c r="I48" t="s">
-        <v>257</v>
-      </c>
-      <c r="J48" t="s">
-        <v>258</v>
-      </c>
-      <c r="K48" t="s">
-        <v>259</v>
-      </c>
-      <c r="L48" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>507</v>
       </c>
@@ -7137,25 +6929,19 @@
         <v>262</v>
       </c>
       <c r="G49" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="H49" t="s">
+        <v>266</v>
+      </c>
+      <c r="I49" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" t="s">
         <v>20</v>
       </c>
-      <c r="I49" t="s">
-        <v>263</v>
-      </c>
-      <c r="J49" t="s">
-        <v>264</v>
-      </c>
-      <c r="K49" t="s">
-        <v>265</v>
-      </c>
-      <c r="L49" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>507</v>
       </c>
@@ -7174,22 +6960,19 @@
         <v>268</v>
       </c>
       <c r="G50" t="s">
-        <v>19</v>
+        <v>269</v>
       </c>
       <c r="H50" t="s">
+        <v>271</v>
+      </c>
+      <c r="I50" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" t="s">
         <v>32</v>
       </c>
-      <c r="I50" t="s">
-        <v>269</v>
-      </c>
-      <c r="J50" t="s">
-        <v>270</v>
-      </c>
-      <c r="L50" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>507</v>
       </c>
@@ -7208,25 +6991,19 @@
         <v>273</v>
       </c>
       <c r="G51" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H51" t="s">
+        <v>276</v>
+      </c>
+      <c r="I51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" t="s">
         <v>20</v>
       </c>
-      <c r="I51" t="s">
-        <v>21</v>
-      </c>
-      <c r="J51" t="s">
-        <v>274</v>
-      </c>
-      <c r="K51" t="s">
-        <v>275</v>
-      </c>
-      <c r="L51" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>507</v>
       </c>
@@ -7244,14 +7021,14 @@
       <c r="F52" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="I52" t="s">
+      <c r="G52" t="s">
         <v>279</v>
       </c>
-      <c r="L52" t="s">
+      <c r="H52" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>528</v>
       </c>
@@ -7270,25 +7047,19 @@
         <v>282</v>
       </c>
       <c r="G53" t="s">
-        <v>19</v>
+        <v>283</v>
       </c>
       <c r="H53" t="s">
+        <v>286</v>
+      </c>
+      <c r="I53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" t="s">
         <v>20</v>
       </c>
-      <c r="I53" t="s">
-        <v>283</v>
-      </c>
-      <c r="J53" t="s">
-        <v>284</v>
-      </c>
-      <c r="K53" t="s">
-        <v>285</v>
-      </c>
-      <c r="L53" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>511</v>
       </c>
@@ -7307,22 +7078,19 @@
         <v>288</v>
       </c>
       <c r="G54" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="H54" t="s">
+        <v>291</v>
+      </c>
+      <c r="I54" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" t="s">
         <v>20</v>
       </c>
-      <c r="I54" t="s">
-        <v>289</v>
-      </c>
-      <c r="K54" t="s">
-        <v>290</v>
-      </c>
-      <c r="L54" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>507</v>
       </c>
@@ -7341,25 +7109,19 @@
         <v>293</v>
       </c>
       <c r="G55" t="s">
-        <v>19</v>
+        <v>222</v>
       </c>
       <c r="H55" t="s">
+        <v>296</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" t="s">
         <v>20</v>
       </c>
-      <c r="I55" t="s">
-        <v>222</v>
-      </c>
-      <c r="J55" t="s">
-        <v>294</v>
-      </c>
-      <c r="K55" t="s">
-        <v>295</v>
-      </c>
-      <c r="L55" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>507</v>
       </c>
@@ -7378,25 +7140,19 @@
         <v>298</v>
       </c>
       <c r="G56" t="s">
-        <v>19</v>
+        <v>299</v>
       </c>
       <c r="H56" t="s">
+        <v>302</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" t="s">
         <v>20</v>
       </c>
-      <c r="I56" t="s">
-        <v>299</v>
-      </c>
-      <c r="J56" t="s">
-        <v>300</v>
-      </c>
-      <c r="K56" t="s">
-        <v>301</v>
-      </c>
-      <c r="L56" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>507</v>
       </c>
@@ -7415,25 +7171,19 @@
         <v>304</v>
       </c>
       <c r="G57" t="s">
+        <v>306</v>
+      </c>
+      <c r="H57" t="s">
+        <v>309</v>
+      </c>
+      <c r="I57" t="s">
         <v>305</v>
       </c>
-      <c r="H57" t="s">
+      <c r="K57" t="s">
         <v>20</v>
       </c>
-      <c r="I57" t="s">
-        <v>306</v>
-      </c>
-      <c r="J57" t="s">
-        <v>307</v>
-      </c>
-      <c r="K57" t="s">
-        <v>308</v>
-      </c>
-      <c r="L57" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>507</v>
       </c>
@@ -7452,22 +7202,19 @@
         <v>311</v>
       </c>
       <c r="G58" t="s">
+        <v>312</v>
+      </c>
+      <c r="H58" t="s">
+        <v>314</v>
+      </c>
+      <c r="I58" t="s">
         <v>256</v>
       </c>
-      <c r="H58" t="s">
+      <c r="K58" t="s">
         <v>20</v>
       </c>
-      <c r="I58" t="s">
-        <v>312</v>
-      </c>
-      <c r="J58" t="s">
-        <v>313</v>
-      </c>
-      <c r="L58" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>507</v>
       </c>
@@ -7486,25 +7233,19 @@
         <v>316</v>
       </c>
       <c r="G59" t="s">
+        <v>317</v>
+      </c>
+      <c r="H59" t="s">
+        <v>320</v>
+      </c>
+      <c r="I59" t="s">
         <v>305</v>
       </c>
-      <c r="H59" t="s">
+      <c r="K59" t="s">
         <v>20</v>
       </c>
-      <c r="I59" t="s">
-        <v>317</v>
-      </c>
-      <c r="J59" t="s">
-        <v>318</v>
-      </c>
-      <c r="K59" t="s">
-        <v>319</v>
-      </c>
-      <c r="L59" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>507</v>
       </c>
@@ -7525,22 +7266,19 @@
         <v>322</v>
       </c>
       <c r="G60" t="s">
+        <v>269</v>
+      </c>
+      <c r="H60" t="s">
+        <v>324</v>
+      </c>
+      <c r="I60" t="s">
         <v>181</v>
       </c>
-      <c r="H60" t="s">
+      <c r="K60" t="s">
         <v>32</v>
       </c>
-      <c r="I60" t="s">
-        <v>269</v>
-      </c>
-      <c r="J60" t="s">
-        <v>323</v>
-      </c>
-      <c r="L60" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>507</v>
       </c>
@@ -7559,25 +7297,19 @@
         <v>326</v>
       </c>
       <c r="G61" t="s">
-        <v>19</v>
+        <v>327</v>
       </c>
       <c r="H61" t="s">
+        <v>330</v>
+      </c>
+      <c r="I61" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" t="s">
         <v>32</v>
       </c>
-      <c r="I61" t="s">
-        <v>327</v>
-      </c>
-      <c r="J61" t="s">
-        <v>328</v>
-      </c>
-      <c r="K61" t="s">
-        <v>329</v>
-      </c>
-      <c r="L61" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>558</v>
       </c>
@@ -7596,25 +7328,19 @@
         <v>332</v>
       </c>
       <c r="G62" t="s">
+        <v>317</v>
+      </c>
+      <c r="H62" t="s">
+        <v>335</v>
+      </c>
+      <c r="I62" t="s">
         <v>305</v>
       </c>
-      <c r="H62" t="s">
+      <c r="K62" t="s">
         <v>20</v>
       </c>
-      <c r="I62" t="s">
-        <v>317</v>
-      </c>
-      <c r="J62" t="s">
-        <v>333</v>
-      </c>
-      <c r="K62" t="s">
-        <v>334</v>
-      </c>
-      <c r="L62" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>507</v>
       </c>
@@ -7633,19 +7359,16 @@
         <v>337</v>
       </c>
       <c r="G63" t="s">
+        <v>338</v>
+      </c>
+      <c r="H63" t="s">
+        <v>340</v>
+      </c>
+      <c r="I63" t="s">
         <v>181</v>
       </c>
-      <c r="I63" t="s">
-        <v>338</v>
-      </c>
-      <c r="K63" t="s">
-        <v>339</v>
-      </c>
-      <c r="L63" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:11" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>507</v>
       </c>
@@ -7664,25 +7387,19 @@
         <v>342</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>343</v>
       </c>
       <c r="H64" t="s">
+        <v>346</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="K64" t="s">
         <v>20</v>
       </c>
-      <c r="I64" t="s">
-        <v>343</v>
-      </c>
-      <c r="J64" t="s">
-        <v>344</v>
-      </c>
-      <c r="K64" t="s">
-        <v>345</v>
-      </c>
-      <c r="L64" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>507</v>
       </c>
@@ -7701,25 +7418,19 @@
         <v>348</v>
       </c>
       <c r="G65" t="s">
+        <v>349</v>
+      </c>
+      <c r="H65" t="s">
+        <v>352</v>
+      </c>
+      <c r="I65" t="s">
         <v>256</v>
       </c>
-      <c r="H65" t="s">
+      <c r="K65" t="s">
         <v>20</v>
       </c>
-      <c r="I65" t="s">
-        <v>349</v>
-      </c>
-      <c r="J65" t="s">
-        <v>350</v>
-      </c>
-      <c r="K65" t="s">
-        <v>351</v>
-      </c>
-      <c r="L65" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>507</v>
       </c>
@@ -7738,25 +7449,19 @@
         <v>354</v>
       </c>
       <c r="G66" t="s">
+        <v>355</v>
+      </c>
+      <c r="H66" t="s">
+        <v>358</v>
+      </c>
+      <c r="I66" t="s">
         <v>181</v>
       </c>
-      <c r="H66" t="s">
+      <c r="K66" t="s">
         <v>20</v>
       </c>
-      <c r="I66" t="s">
-        <v>355</v>
-      </c>
-      <c r="J66" t="s">
-        <v>356</v>
-      </c>
-      <c r="K66" t="s">
-        <v>357</v>
-      </c>
-      <c r="L66" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>507</v>
       </c>
@@ -7775,25 +7480,19 @@
         <v>360</v>
       </c>
       <c r="G67" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="H67" t="s">
+        <v>363</v>
+      </c>
+      <c r="I67" t="s">
+        <v>19</v>
+      </c>
+      <c r="K67" t="s">
         <v>32</v>
       </c>
-      <c r="I67" t="s">
-        <v>95</v>
-      </c>
-      <c r="J67" t="s">
-        <v>361</v>
-      </c>
-      <c r="K67" t="s">
-        <v>362</v>
-      </c>
-      <c r="L67" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>507</v>
       </c>
@@ -7812,25 +7511,19 @@
         <v>365</v>
       </c>
       <c r="G68" t="s">
+        <v>366</v>
+      </c>
+      <c r="H68" t="s">
+        <v>369</v>
+      </c>
+      <c r="I68" t="s">
         <v>256</v>
       </c>
-      <c r="H68" t="s">
+      <c r="K68" t="s">
         <v>32</v>
       </c>
-      <c r="I68" t="s">
-        <v>366</v>
-      </c>
-      <c r="J68" t="s">
-        <v>367</v>
-      </c>
-      <c r="K68" t="s">
-        <v>368</v>
-      </c>
-      <c r="L68" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>507</v>
       </c>
@@ -7849,25 +7542,19 @@
         <v>371</v>
       </c>
       <c r="G69" t="s">
-        <v>19</v>
+        <v>372</v>
       </c>
       <c r="H69" t="s">
+        <v>375</v>
+      </c>
+      <c r="I69" t="s">
+        <v>19</v>
+      </c>
+      <c r="K69" t="s">
         <v>20</v>
       </c>
-      <c r="I69" t="s">
-        <v>372</v>
-      </c>
-      <c r="J69" t="s">
-        <v>373</v>
-      </c>
-      <c r="K69" t="s">
-        <v>374</v>
-      </c>
-      <c r="L69" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>507</v>
       </c>
@@ -7886,16 +7573,16 @@
         <v>377</v>
       </c>
       <c r="G70" t="s">
+        <v>246</v>
+      </c>
+      <c r="H70" t="s">
+        <v>378</v>
+      </c>
+      <c r="I70" t="s">
         <v>305</v>
       </c>
-      <c r="I70" t="s">
-        <v>246</v>
-      </c>
-      <c r="L70" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>507</v>
       </c>
@@ -7914,25 +7601,19 @@
         <v>380</v>
       </c>
       <c r="G71" t="s">
+        <v>381</v>
+      </c>
+      <c r="H71" t="s">
+        <v>384</v>
+      </c>
+      <c r="I71" t="s">
         <v>305</v>
       </c>
-      <c r="H71" t="s">
+      <c r="K71" t="s">
         <v>20</v>
       </c>
-      <c r="I71" t="s">
-        <v>381</v>
-      </c>
-      <c r="J71" t="s">
-        <v>382</v>
-      </c>
-      <c r="K71" t="s">
-        <v>383</v>
-      </c>
-      <c r="L71" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>516</v>
       </c>
@@ -7953,13 +7634,13 @@
         <v>386</v>
       </c>
       <c r="G72" t="s">
+        <v>269</v>
+      </c>
+      <c r="I72" t="s">
         <v>181</v>
       </c>
-      <c r="I72" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>507</v>
       </c>
@@ -7978,25 +7659,19 @@
         <v>388</v>
       </c>
       <c r="G73" t="s">
-        <v>19</v>
+        <v>389</v>
       </c>
       <c r="H73" t="s">
+        <v>392</v>
+      </c>
+      <c r="I73" t="s">
+        <v>19</v>
+      </c>
+      <c r="K73" t="s">
         <v>32</v>
       </c>
-      <c r="I73" t="s">
-        <v>389</v>
-      </c>
-      <c r="J73" t="s">
-        <v>390</v>
-      </c>
-      <c r="K73" t="s">
-        <v>391</v>
-      </c>
-      <c r="L73" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>507</v>
       </c>
@@ -8015,25 +7690,19 @@
         <v>394</v>
       </c>
       <c r="G74" t="s">
-        <v>19</v>
+        <v>395</v>
       </c>
       <c r="H74" t="s">
+        <v>398</v>
+      </c>
+      <c r="I74" t="s">
+        <v>19</v>
+      </c>
+      <c r="K74" t="s">
         <v>32</v>
       </c>
-      <c r="I74" t="s">
-        <v>395</v>
-      </c>
-      <c r="J74" t="s">
-        <v>396</v>
-      </c>
-      <c r="K74" t="s">
-        <v>397</v>
-      </c>
-      <c r="L74" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>507</v>
       </c>
@@ -8052,25 +7721,19 @@
         <v>400</v>
       </c>
       <c r="G75" t="s">
-        <v>19</v>
+        <v>401</v>
       </c>
       <c r="H75" t="s">
+        <v>404</v>
+      </c>
+      <c r="I75" t="s">
+        <v>19</v>
+      </c>
+      <c r="K75" t="s">
         <v>32</v>
       </c>
-      <c r="I75" t="s">
-        <v>401</v>
-      </c>
-      <c r="J75" t="s">
-        <v>402</v>
-      </c>
-      <c r="K75" t="s">
-        <v>403</v>
-      </c>
-      <c r="L75" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>507</v>
       </c>
@@ -8089,25 +7752,19 @@
         <v>406</v>
       </c>
       <c r="G76" t="s">
-        <v>19</v>
+        <v>407</v>
       </c>
       <c r="H76" t="s">
+        <v>410</v>
+      </c>
+      <c r="I76" t="s">
+        <v>19</v>
+      </c>
+      <c r="K76" t="s">
         <v>20</v>
       </c>
-      <c r="I76" t="s">
-        <v>407</v>
-      </c>
-      <c r="J76" t="s">
-        <v>408</v>
-      </c>
-      <c r="K76" t="s">
-        <v>409</v>
-      </c>
-      <c r="L76" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>528</v>
       </c>
@@ -8126,25 +7783,19 @@
         <v>412</v>
       </c>
       <c r="G77" t="s">
+        <v>283</v>
+      </c>
+      <c r="H77" t="s">
+        <v>346</v>
+      </c>
+      <c r="I77" t="s">
         <v>256</v>
       </c>
-      <c r="H77" t="s">
+      <c r="K77" t="s">
         <v>20</v>
       </c>
-      <c r="I77" t="s">
-        <v>283</v>
-      </c>
-      <c r="J77" t="s">
-        <v>413</v>
-      </c>
-      <c r="K77" t="s">
-        <v>414</v>
-      </c>
-      <c r="L77" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>507</v>
       </c>
@@ -8163,25 +7814,19 @@
         <v>416</v>
       </c>
       <c r="G78" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H78" t="s">
+        <v>419</v>
+      </c>
+      <c r="I78" t="s">
+        <v>19</v>
+      </c>
+      <c r="K78" t="s">
         <v>20</v>
       </c>
-      <c r="I78" t="s">
-        <v>21</v>
-      </c>
-      <c r="J78" t="s">
-        <v>417</v>
-      </c>
-      <c r="K78" t="s">
-        <v>418</v>
-      </c>
-      <c r="L78" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>507</v>
       </c>
@@ -8200,25 +7845,19 @@
         <v>421</v>
       </c>
       <c r="G79" t="s">
-        <v>19</v>
+        <v>422</v>
       </c>
       <c r="H79" t="s">
+        <v>425</v>
+      </c>
+      <c r="I79" t="s">
+        <v>19</v>
+      </c>
+      <c r="K79" t="s">
         <v>20</v>
       </c>
-      <c r="I79" t="s">
-        <v>422</v>
-      </c>
-      <c r="J79" t="s">
-        <v>423</v>
-      </c>
-      <c r="K79" t="s">
-        <v>424</v>
-      </c>
-      <c r="L79" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>507</v>
       </c>
@@ -8236,14 +7875,14 @@
       <c r="F80" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="I80" t="s">
+      <c r="G80" t="s">
         <v>428</v>
       </c>
-      <c r="L80" t="s">
+      <c r="H80" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>507</v>
       </c>
@@ -8262,25 +7901,19 @@
         <v>431</v>
       </c>
       <c r="G81" t="s">
+        <v>432</v>
+      </c>
+      <c r="H81" t="s">
+        <v>435</v>
+      </c>
+      <c r="I81" t="s">
         <v>59</v>
       </c>
-      <c r="H81" t="s">
+      <c r="K81" t="s">
         <v>20</v>
       </c>
-      <c r="I81" t="s">
-        <v>432</v>
-      </c>
-      <c r="J81" t="s">
-        <v>433</v>
-      </c>
-      <c r="K81" t="s">
-        <v>434</v>
-      </c>
-      <c r="L81" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>507</v>
       </c>
@@ -8299,25 +7932,19 @@
         <v>437</v>
       </c>
       <c r="G82" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="H82" t="s">
+        <v>440</v>
+      </c>
+      <c r="I82" t="s">
+        <v>19</v>
+      </c>
+      <c r="K82" t="s">
         <v>20</v>
       </c>
-      <c r="I82" t="s">
-        <v>101</v>
-      </c>
-      <c r="J82" t="s">
-        <v>438</v>
-      </c>
-      <c r="K82" t="s">
-        <v>439</v>
-      </c>
-      <c r="L82" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>507</v>
       </c>
@@ -8336,25 +7963,19 @@
         <v>442</v>
       </c>
       <c r="G83" t="s">
+        <v>443</v>
+      </c>
+      <c r="H83" t="s">
+        <v>446</v>
+      </c>
+      <c r="I83" t="s">
         <v>59</v>
       </c>
-      <c r="H83" t="s">
+      <c r="K83" t="s">
         <v>20</v>
       </c>
-      <c r="I83" t="s">
-        <v>443</v>
-      </c>
-      <c r="J83" t="s">
-        <v>444</v>
-      </c>
-      <c r="K83" t="s">
-        <v>445</v>
-      </c>
-      <c r="L83" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>558</v>
       </c>
@@ -8373,25 +7994,19 @@
         <v>448</v>
       </c>
       <c r="G84" t="s">
-        <v>19</v>
+        <v>263</v>
       </c>
       <c r="H84" t="s">
+        <v>451</v>
+      </c>
+      <c r="I84" t="s">
+        <v>19</v>
+      </c>
+      <c r="K84" t="s">
         <v>20</v>
       </c>
-      <c r="I84" t="s">
-        <v>263</v>
-      </c>
-      <c r="J84" t="s">
-        <v>449</v>
-      </c>
-      <c r="K84" t="s">
-        <v>450</v>
-      </c>
-      <c r="L84" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>507</v>
       </c>
@@ -8409,14 +8024,14 @@
       <c r="F85" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="I85" t="s">
+      <c r="G85" t="s">
         <v>454</v>
       </c>
-      <c r="L85" t="s">
+      <c r="H85" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>507</v>
       </c>
@@ -8435,25 +8050,19 @@
         <v>457</v>
       </c>
       <c r="G86" t="s">
+        <v>458</v>
+      </c>
+      <c r="H86" t="s">
+        <v>461</v>
+      </c>
+      <c r="I86" t="s">
         <v>305</v>
       </c>
-      <c r="H86" t="s">
+      <c r="K86" t="s">
         <v>20</v>
       </c>
-      <c r="I86" t="s">
-        <v>458</v>
-      </c>
-      <c r="J86" t="s">
-        <v>459</v>
-      </c>
-      <c r="K86" t="s">
-        <v>460</v>
-      </c>
-      <c r="L86" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>507</v>
       </c>
@@ -8472,25 +8081,19 @@
         <v>463</v>
       </c>
       <c r="G87" t="s">
+        <v>464</v>
+      </c>
+      <c r="H87" t="s">
+        <v>467</v>
+      </c>
+      <c r="I87" t="s">
         <v>181</v>
       </c>
-      <c r="H87" t="s">
+      <c r="K87" t="s">
         <v>20</v>
       </c>
-      <c r="I87" t="s">
-        <v>464</v>
-      </c>
-      <c r="J87" t="s">
-        <v>465</v>
-      </c>
-      <c r="K87" t="s">
-        <v>466</v>
-      </c>
-      <c r="L87" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>507</v>
       </c>
@@ -8509,25 +8112,19 @@
         <v>469</v>
       </c>
       <c r="G88" t="s">
+        <v>470</v>
+      </c>
+      <c r="H88" t="s">
+        <v>473</v>
+      </c>
+      <c r="I88" t="s">
         <v>181</v>
       </c>
-      <c r="H88" t="s">
+      <c r="K88" t="s">
         <v>32</v>
       </c>
-      <c r="I88" t="s">
-        <v>470</v>
-      </c>
-      <c r="J88" t="s">
-        <v>471</v>
-      </c>
-      <c r="K88" t="s">
-        <v>472</v>
-      </c>
-      <c r="L88" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>507</v>
       </c>
@@ -8546,25 +8143,19 @@
         <v>475</v>
       </c>
       <c r="G89" t="s">
+        <v>476</v>
+      </c>
+      <c r="H89" t="s">
+        <v>479</v>
+      </c>
+      <c r="I89" t="s">
         <v>256</v>
       </c>
-      <c r="H89" t="s">
+      <c r="K89" t="s">
         <v>20</v>
       </c>
-      <c r="I89" t="s">
-        <v>476</v>
-      </c>
-      <c r="J89" t="s">
-        <v>477</v>
-      </c>
-      <c r="K89" t="s">
-        <v>478</v>
-      </c>
-      <c r="L89" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>507</v>
       </c>
@@ -8583,25 +8174,19 @@
         <v>481</v>
       </c>
       <c r="G90" t="s">
-        <v>19</v>
+        <v>389</v>
       </c>
       <c r="H90" t="s">
+        <v>484</v>
+      </c>
+      <c r="I90" t="s">
+        <v>19</v>
+      </c>
+      <c r="K90" t="s">
         <v>32</v>
       </c>
-      <c r="I90" t="s">
-        <v>389</v>
-      </c>
-      <c r="J90" t="s">
-        <v>482</v>
-      </c>
-      <c r="K90" t="s">
-        <v>483</v>
-      </c>
-      <c r="L90" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>507</v>
       </c>
@@ -8620,25 +8205,19 @@
         <v>486</v>
       </c>
       <c r="G91" t="s">
-        <v>19</v>
+        <v>389</v>
       </c>
       <c r="H91" t="s">
+        <v>489</v>
+      </c>
+      <c r="I91" t="s">
+        <v>19</v>
+      </c>
+      <c r="K91" t="s">
         <v>32</v>
       </c>
-      <c r="I91" t="s">
-        <v>389</v>
-      </c>
-      <c r="J91" t="s">
-        <v>487</v>
-      </c>
-      <c r="K91" t="s">
-        <v>488</v>
-      </c>
-      <c r="L91" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>507</v>
       </c>
@@ -8657,25 +8236,19 @@
         <v>491</v>
       </c>
       <c r="G92" t="s">
+        <v>493</v>
+      </c>
+      <c r="H92" t="s">
+        <v>496</v>
+      </c>
+      <c r="I92" t="s">
         <v>492</v>
       </c>
-      <c r="H92" t="s">
+      <c r="K92" t="s">
         <v>20</v>
       </c>
-      <c r="I92" t="s">
-        <v>493</v>
-      </c>
-      <c r="J92" t="s">
-        <v>494</v>
-      </c>
-      <c r="K92" t="s">
-        <v>495</v>
-      </c>
-      <c r="L92" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>507</v>
       </c>
@@ -8694,25 +8267,19 @@
         <v>498</v>
       </c>
       <c r="G93" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H93" t="s">
+        <v>501</v>
+      </c>
+      <c r="I93" t="s">
+        <v>19</v>
+      </c>
+      <c r="K93" t="s">
         <v>20</v>
       </c>
-      <c r="I93" t="s">
-        <v>21</v>
-      </c>
-      <c r="J93" t="s">
-        <v>499</v>
-      </c>
-      <c r="K93" t="s">
-        <v>500</v>
-      </c>
-      <c r="L93" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>507</v>
       </c>
@@ -8731,32 +8298,20 @@
         <v>503</v>
       </c>
       <c r="G94" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H94" t="s">
+        <v>506</v>
+      </c>
+      <c r="I94" t="s">
+        <v>19</v>
+      </c>
+      <c r="K94" t="s">
         <v>20</v>
       </c>
-      <c r="I94" t="s">
-        <v>21</v>
-      </c>
-      <c r="J94" t="s">
-        <v>504</v>
-      </c>
-      <c r="K94" t="s">
-        <v>505</v>
-      </c>
-      <c r="L94" t="s">
-        <v>506</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N94" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="OK"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K94" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8765,403 +8320,403 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68E7F53-D341-42A1-8716-BC7EA4877C31}">
   <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection sqref="A1:A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="210" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="225" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="195" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>502</v>
       </c>

</xml_diff>